<commit_message>
Work on Dashboard and Report
</commit_message>
<xml_diff>
--- a/Report/Seoul Bike Analysis.xlsx
+++ b/Report/Seoul Bike Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\Seoul Bike Analysis\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33EA3CFB-3235-4EB8-B8C8-C4DB678E39BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A589487-1D6A-4267-B663-5C688CBD7ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{846708F6-76B2-4DF5-BE10-DAA347BD8AC3}"/>
   </bookViews>
@@ -429,12 +429,6 @@
     <t>Shows at which temperature range each season performs best.</t>
   </si>
   <si>
-    <t>Season + Temperature Heatmap</t>
-  </si>
-  <si>
-    <t>Hour vs Day Name (Heatmap)</t>
-  </si>
-  <si>
     <t>Correlation Visualization (Scatter)</t>
   </si>
   <si>
@@ -466,6 +460,12 @@
   </si>
   <si>
     <t>See if any data gaps or day impact.</t>
+  </si>
+  <si>
+    <t>Season + Temperature</t>
+  </si>
+  <si>
+    <t>Hour vs Day Name</t>
   </si>
 </sst>
 </file>
@@ -1785,8 +1785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8555E78B-340A-479A-93F3-D407999AA8F3}">
   <dimension ref="B2:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2148,7 +2148,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="F19" s="37" t="s">
         <v>128</v>
@@ -2165,16 +2165,16 @@
         <v>2</v>
       </c>
       <c r="E20" s="35" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="F20" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="G20" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="H20" s="37" t="s">
         <v>134</v>
-      </c>
-      <c r="G20" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="H20" s="37" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="21" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
@@ -2182,16 +2182,16 @@
         <v>3</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F21" s="37" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G21" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="H21" s="37" t="s">
         <v>137</v>
-      </c>
-      <c r="H21" s="37" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="22" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
@@ -2199,16 +2199,16 @@
         <v>4</v>
       </c>
       <c r="E22" s="35" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F22" s="37" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G22" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="H22" s="37" t="s">
         <v>140</v>
-      </c>
-      <c r="H22" s="37" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete the work of report Excel,PDF,Word These format are included
</commit_message>
<xml_diff>
--- a/Report/Seoul Bike Analysis.xlsx
+++ b/Report/Seoul Bike Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\Seoul Bike Analysis\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A589487-1D6A-4267-B663-5C688CBD7ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8498A19-B915-47AC-857C-C9C32048F67C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{846708F6-76B2-4DF5-BE10-DAA347BD8AC3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{846708F6-76B2-4DF5-BE10-DAA347BD8AC3}"/>
   </bookViews>
   <sheets>
     <sheet name="KYV Column" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="144">
   <si>
     <t>Know Your Value/Column</t>
   </si>
@@ -372,18 +372,9 @@
     <t>Hour, SUM(Bike_Count)</t>
   </si>
   <si>
-    <t>Calculated column (Rainy / Clear)</t>
-  </si>
-  <si>
     <t>Month</t>
   </si>
   <si>
-    <t>Day</t>
-  </si>
-  <si>
-    <t>Weather Type</t>
-  </si>
-  <si>
     <t>SUM([Bike_Count])</t>
   </si>
   <si>
@@ -466,6 +457,131 @@
   </si>
   <si>
     <t>Hour vs Day Name</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This column shows the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name of the day</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for each date (like Monday, Tuesday, etc.).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This column shows the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>month name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for each date (like January, February, etc.).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This column shows the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>year</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of each record.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This column tells whether a day is a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Weekday</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Monday–Friday) or a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Weekend</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Saturday–Sunday).</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -576,7 +692,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -631,6 +747,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -659,7 +787,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -727,9 +855,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -757,6 +883,14 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1074,19 +1208,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA3A81E-0245-4107-9F9B-2C1ADAEFD483}">
   <dimension ref="B3:H23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="39" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:G23"/>
+    <sheetView tabSelected="1" zoomScale="43" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" customWidth="1"/>
     <col min="3" max="3" width="28.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.44140625" customWidth="1"/>
     <col min="5" max="5" width="41.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.77734375" customWidth="1"/>
     <col min="7" max="7" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="50.77734375" customWidth="1"/>
+    <col min="8" max="8" width="84.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="25.8" x14ac:dyDescent="0.5">
@@ -1102,7 +1236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1138,7 +1272,9 @@
       <c r="G7" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="H7" s="22"/>
+      <c r="H7" s="20" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B8" s="18">
@@ -1156,7 +1292,9 @@
       <c r="G8" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="22"/>
+      <c r="H8" s="20" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="9" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B9" s="18">
@@ -1174,7 +1312,9 @@
       <c r="G9" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="22"/>
+      <c r="H9" s="20" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B10" s="18">
@@ -1192,7 +1332,9 @@
       <c r="G10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="22"/>
+      <c r="H10" s="20" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="11" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B11" s="18">
@@ -1210,7 +1352,9 @@
       <c r="G11" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="H11" s="22"/>
+      <c r="H11" s="20" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="12" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B12" s="18">
@@ -1228,7 +1372,9 @@
       <c r="G12" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="H12" s="22"/>
+      <c r="H12" s="20" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="13" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B13" s="18">
@@ -1246,7 +1392,9 @@
       <c r="G13" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="H13" s="22"/>
+      <c r="H13" s="20" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="14" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B14" s="18">
@@ -1264,7 +1412,9 @@
       <c r="G14" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="H14" s="22"/>
+      <c r="H14" s="20" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="15" spans="2:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B15" s="18">
@@ -1282,7 +1432,9 @@
       <c r="G15" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="H15" s="22"/>
+      <c r="H15" s="20" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="16" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B16" s="18">
@@ -1300,7 +1452,9 @@
       <c r="G16" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="H16" s="22"/>
+      <c r="H16" s="20" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="17" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B17" s="18">
@@ -1318,7 +1472,9 @@
       <c r="G17" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="H17" s="22"/>
+      <c r="H17" s="20" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="18" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B18" s="18">
@@ -1336,7 +1492,9 @@
       <c r="G18" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="H18" s="22"/>
+      <c r="H18" s="20" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="19" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B19" s="18">
@@ -1354,7 +1512,9 @@
       <c r="G19" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="H19" s="22"/>
+      <c r="H19" s="20" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="20" spans="2:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B20" s="18">
@@ -1369,10 +1529,12 @@
       <c r="F20" s="21">
         <v>14</v>
       </c>
-      <c r="G20" s="26" t="s">
+      <c r="G20" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="H20" s="23"/>
+      <c r="H20" s="39" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="21" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="F21" s="21">
@@ -1381,25 +1543,31 @@
       <c r="G21" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="H21" s="23"/>
+      <c r="H21" s="39" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="22" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="F22" s="21">
         <v>16</v>
       </c>
-      <c r="G22" s="26" t="s">
+      <c r="G22" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="H22" s="23"/>
+      <c r="H22" s="39" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F23" s="24">
         <v>17</v>
       </c>
-      <c r="G23" s="27" t="s">
+      <c r="G23" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="H23" s="25"/>
+      <c r="H23" s="39" t="s">
+        <v>143</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1408,16 +1576,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BBB1CA9-1A74-481D-BE6F-A12BD82377E2}">
-  <dimension ref="B2:K14"/>
+  <dimension ref="B2:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -1463,300 +1631,293 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5">
+    <row r="5" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B5" s="23">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="23">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="23">
         <v>8760</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="23">
         <v>8760</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="36">
         <v>0</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="23">
         <v>14</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="23">
         <v>14</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6">
+    <row r="6" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="23">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="23">
         <v>2</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="23">
         <f t="shared" ref="F6:F13" si="0">G5</f>
         <v>8760</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="23">
         <v>8760</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="36">
         <v>0</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="23">
         <v>14</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="23">
         <v>14</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7">
+    <row r="7" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="23">
         <v>3</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="23">
         <v>3</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="23">
         <f t="shared" si="0"/>
         <v>8760</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="23">
         <v>8760</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="36">
         <v>0</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="23">
         <v>14</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="23">
         <v>14</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8">
+    <row r="8" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="23">
         <v>4</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="23">
         <v>4</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="23">
         <f t="shared" si="0"/>
         <v>8760</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="23">
         <v>8760</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="36">
         <v>0</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="23">
         <v>14</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="23">
         <v>14</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9">
+    <row r="9" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="23">
         <v>5</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="23">
         <v>5</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="23">
         <f t="shared" si="0"/>
         <v>8760</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="23">
         <v>8760</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="36">
         <v>0</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="23">
         <v>14</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="23">
         <v>13</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="37">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10">
+    <row r="10" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="23">
         <v>6</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="23">
         <v>6</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="23">
         <f t="shared" si="0"/>
         <v>8760</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="23">
         <v>8760</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="36">
         <v>0</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="23">
         <v>13</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="23">
         <v>14</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="37">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11">
+    <row r="11" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="23">
         <v>7</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="23">
         <v>7</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="23">
         <f t="shared" si="0"/>
         <v>8760</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="23">
         <v>8760</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="36">
         <v>0</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="23">
         <v>14</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="23">
         <v>15</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="37">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12">
+    <row r="12" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B12" s="23">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="23">
         <v>8</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="23">
         <f t="shared" si="0"/>
         <v>8760</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="23">
         <v>8760</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="36">
         <v>0</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="23">
         <v>15</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="23">
         <v>16</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="37">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13">
+    <row r="13" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B13" s="23">
         <v>9</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="23">
         <v>9</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="23">
         <f t="shared" si="0"/>
         <v>8760</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="23">
         <v>8760</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="36">
         <v>0</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="23">
         <v>16</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="23">
         <v>17</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="37">
         <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14">
-        <v>10</v>
-      </c>
-      <c r="E14">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93BE4181-B463-4FE1-8EC0-37C97001E8A0}">
-  <dimension ref="B2:D4"/>
+  <dimension ref="B2:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="B2" sqref="B2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1774,6 +1935,61 @@
       </c>
       <c r="D4" s="4" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B5" s="23">
+        <v>1</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="23">
+        <v>2</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="23">
+        <v>3</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="23">
+        <v>4</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="23">
+        <v>5</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1785,8 +2001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8555E78B-340A-479A-93F3-D407999AA8F3}">
   <dimension ref="B2:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1814,8 +2030,8 @@
       </c>
     </row>
     <row r="4" spans="2:19" s="12" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B4" s="36" t="s">
-        <v>125</v>
+      <c r="B4" s="34" t="s">
+        <v>122</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="15" t="s">
@@ -1867,250 +2083,214 @@
       </c>
     </row>
     <row r="7" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D7" s="29">
+      <c r="D7" s="27">
         <v>1</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="F7" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="G7" s="32" t="s">
-        <v>115</v>
+      <c r="F7" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>112</v>
       </c>
       <c r="J7" s="23">
         <v>1</v>
       </c>
-      <c r="K7" s="31" t="s">
+      <c r="K7" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="L7" s="28" t="s">
+      <c r="L7" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="M7" s="29" t="s">
+      <c r="M7" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="N7" s="30" t="s">
+      <c r="N7" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="Q7" s="34">
+      <c r="Q7" s="32">
         <v>1</v>
       </c>
-      <c r="R7" s="33" t="s">
+      <c r="R7" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="S7" s="32" t="s">
+      <c r="S7" s="30" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="8" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D8" s="29">
+      <c r="D8" s="27">
         <v>2</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="G8" s="32" t="s">
-        <v>116</v>
+      <c r="F8" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>113</v>
       </c>
       <c r="J8" s="23">
         <v>2</v>
       </c>
-      <c r="K8" s="31" t="s">
+      <c r="K8" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="L8" s="30" t="s">
+      <c r="L8" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="M8" s="30" t="s">
+      <c r="M8" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="N8" s="30" t="s">
+      <c r="N8" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="Q8" s="34">
+      <c r="Q8" s="32">
         <v>2</v>
       </c>
-      <c r="R8" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="S8" s="32" t="s">
-        <v>75</v>
+      <c r="R8" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="S8" s="30" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D9" s="29">
+      <c r="D9" s="27">
         <v>3</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="G9" s="32" t="s">
-        <v>117</v>
+      <c r="F9" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>114</v>
       </c>
       <c r="J9" s="23">
         <v>3</v>
       </c>
-      <c r="K9" s="31" t="s">
+      <c r="K9" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="L9" s="30" t="s">
+      <c r="L9" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="N9" s="30" t="s">
+      <c r="N9" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="Q9" s="34">
+      <c r="Q9" s="32">
         <v>3</v>
       </c>
-      <c r="R9" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="S9" s="32" t="s">
+      <c r="R9" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="S9" s="30" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="10" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D10" s="29">
+      <c r="D10" s="27">
         <v>4</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="F10" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="G10" s="32" t="s">
-        <v>118</v>
+      <c r="F10" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>115</v>
       </c>
       <c r="J10" s="23">
         <v>4</v>
       </c>
-      <c r="K10" s="31" t="s">
+      <c r="K10" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="L10" s="30" t="s">
+      <c r="L10" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="M10" s="30" t="s">
+      <c r="M10" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="N10" s="30" t="s">
+      <c r="N10" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="Q10" s="34">
-        <v>4</v>
-      </c>
-      <c r="R10" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="S10" s="32" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="11" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D11" s="29">
+      <c r="D11" s="27">
         <v>5</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="F11" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="G11" s="32" t="s">
-        <v>119</v>
+      <c r="F11" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>116</v>
       </c>
       <c r="J11" s="23">
         <v>5</v>
       </c>
-      <c r="K11" s="31" t="s">
+      <c r="K11" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="L11" s="30" t="s">
+      <c r="L11" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="M11" s="30" t="s">
+      <c r="M11" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="N11" s="30" t="s">
+      <c r="N11" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="Q11" s="34">
-        <v>5</v>
-      </c>
-      <c r="R11" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="S11" s="32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="2:19" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J12" s="23">
         <v>6</v>
       </c>
-      <c r="K12" s="31" t="s">
+      <c r="K12" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="L12" s="30" t="s">
+      <c r="L12" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="M12" s="30" t="s">
+      <c r="M12" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="N12" s="30" t="s">
+      <c r="N12" s="28" t="s">
         <v>107</v>
-      </c>
-      <c r="Q12" s="34">
-        <v>6</v>
-      </c>
-      <c r="R12" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="S12" s="32" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="13" spans="2:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="J13" s="23">
         <v>7</v>
       </c>
-      <c r="K13" s="31" t="s">
+      <c r="K13" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="L13" s="30" t="s">
+      <c r="L13" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="M13" s="30" t="s">
+      <c r="M13" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="N13" s="30" t="s">
+      <c r="N13" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="Q13" s="34">
-        <v>7</v>
-      </c>
-      <c r="R13" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="S13" s="32" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="16" spans="2:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B16" s="36" t="s">
-        <v>126</v>
+      <c r="B16" s="34" t="s">
+        <v>123</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="16" t="s">
@@ -2144,71 +2324,71 @@
       <c r="O18" s="12"/>
     </row>
     <row r="19" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D19" s="29">
+      <c r="D19" s="27">
         <v>1</v>
       </c>
-      <c r="E19" s="35" t="s">
-        <v>141</v>
-      </c>
-      <c r="F19" s="37" t="s">
+      <c r="E19" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="G19" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="H19" s="35" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D20" s="27">
+        <v>2</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="G20" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="H20" s="35" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D21" s="27">
+        <v>3</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="F21" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="G21" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="H21" s="35" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D22" s="27">
+        <v>4</v>
+      </c>
+      <c r="E22" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="G19" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="H19" s="37" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D20" s="29">
-        <v>2</v>
-      </c>
-      <c r="E20" s="35" t="s">
-        <v>142</v>
-      </c>
-      <c r="F20" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="G20" s="37" t="s">
-        <v>133</v>
-      </c>
-      <c r="H20" s="37" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="21" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D21" s="29">
-        <v>3</v>
-      </c>
-      <c r="E21" s="35" t="s">
-        <v>130</v>
-      </c>
-      <c r="F21" s="37" t="s">
+      <c r="F22" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="G21" s="37" t="s">
+      <c r="G22" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="H21" s="37" t="s">
+      <c r="H22" s="35" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="22" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D22" s="29">
-        <v>4</v>
-      </c>
-      <c r="E22" s="35" t="s">
-        <v>131</v>
-      </c>
-      <c r="F22" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="G22" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="H22" s="37" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>